<commit_message>
Initial support for Ardupilot dataflash log (.bin) files
</commit_message>
<xml_diff>
--- a/Channel Mapping.xlsx
+++ b/Channel Mapping.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Repositories\RadioControl\RCLogAnalyzer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Repositories\RadioControl\RCLogViewer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59DCD20-1E0E-45F3-97B7-1018E6C9F9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F3BF32-B2AE-4BBA-96A9-389DF747703D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{0409232D-7A61-4A3C-AC38-8C0B8237B97C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{0409232D-7A61-4A3C-AC38-8C0B8237B97C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="CSV Files" sheetId="1" r:id="rId1"/>
+    <sheet name="bin File Messages" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="316">
   <si>
     <t>Date</t>
   </si>
@@ -280,6 +281,711 @@
   </si>
   <si>
     <t>Mapping Text</t>
+  </si>
+  <si>
+    <t>ACC1</t>
+  </si>
+  <si>
+    <t>ACC2</t>
+  </si>
+  <si>
+    <t>ACC3</t>
+  </si>
+  <si>
+    <t>ADSB</t>
+  </si>
+  <si>
+    <t>AETR</t>
+  </si>
+  <si>
+    <t>AHR2</t>
+  </si>
+  <si>
+    <t>AOA</t>
+  </si>
+  <si>
+    <t>ARM</t>
+  </si>
+  <si>
+    <t>ARSP</t>
+  </si>
+  <si>
+    <t>ASP2</t>
+  </si>
+  <si>
+    <t>ATRP</t>
+  </si>
+  <si>
+    <t>ATT</t>
+  </si>
+  <si>
+    <t>BAR2</t>
+  </si>
+  <si>
+    <t>BAR3</t>
+  </si>
+  <si>
+    <t>BARO</t>
+  </si>
+  <si>
+    <t>BAT</t>
+  </si>
+  <si>
+    <t>BAT2</t>
+  </si>
+  <si>
+    <t>BAT3</t>
+  </si>
+  <si>
+    <t>BAT4</t>
+  </si>
+  <si>
+    <t>BAT5</t>
+  </si>
+  <si>
+    <t>BAT6</t>
+  </si>
+  <si>
+    <t>BAT7</t>
+  </si>
+  <si>
+    <t>BAT8</t>
+  </si>
+  <si>
+    <t>BAT9</t>
+  </si>
+  <si>
+    <t>BCL</t>
+  </si>
+  <si>
+    <t>BCL2</t>
+  </si>
+  <si>
+    <t>BCL3</t>
+  </si>
+  <si>
+    <t>BCL4</t>
+  </si>
+  <si>
+    <t>BCL5</t>
+  </si>
+  <si>
+    <t>BCL6</t>
+  </si>
+  <si>
+    <t>BCL7</t>
+  </si>
+  <si>
+    <t>BCL8</t>
+  </si>
+  <si>
+    <t>BCL9</t>
+  </si>
+  <si>
+    <t>BCN</t>
+  </si>
+  <si>
+    <t>CAM</t>
+  </si>
+  <si>
+    <t>CESC</t>
+  </si>
+  <si>
+    <t>CMD</t>
+  </si>
+  <si>
+    <t>CSRV</t>
+  </si>
+  <si>
+    <t>CTUN</t>
+  </si>
+  <si>
+    <t>DMS</t>
+  </si>
+  <si>
+    <t>DSF</t>
+  </si>
+  <si>
+    <t>DSTL</t>
+  </si>
+  <si>
+    <t>ERR</t>
+  </si>
+  <si>
+    <t>ESC1</t>
+  </si>
+  <si>
+    <t>ESC2</t>
+  </si>
+  <si>
+    <t>ESC3</t>
+  </si>
+  <si>
+    <t>ESC4</t>
+  </si>
+  <si>
+    <t>ESC5</t>
+  </si>
+  <si>
+    <t>ESC6</t>
+  </si>
+  <si>
+    <t>ESC7</t>
+  </si>
+  <si>
+    <t>ESC8</t>
+  </si>
+  <si>
+    <t>EV</t>
+  </si>
+  <si>
+    <t>FMT</t>
+  </si>
+  <si>
+    <t>FMTU</t>
+  </si>
+  <si>
+    <t>GMB1</t>
+  </si>
+  <si>
+    <t>GMB2</t>
+  </si>
+  <si>
+    <t>GMB3</t>
+  </si>
+  <si>
+    <t>GPA</t>
+  </si>
+  <si>
+    <t>GPA2</t>
+  </si>
+  <si>
+    <t>GPAB</t>
+  </si>
+  <si>
+    <t>GPS2</t>
+  </si>
+  <si>
+    <t>GPSB</t>
+  </si>
+  <si>
+    <t>GRAW</t>
+  </si>
+  <si>
+    <t>GRXH</t>
+  </si>
+  <si>
+    <t>GRXS</t>
+  </si>
+  <si>
+    <t>GYR1</t>
+  </si>
+  <si>
+    <t>GYR2</t>
+  </si>
+  <si>
+    <t>GYR3</t>
+  </si>
+  <si>
+    <t>IMT</t>
+  </si>
+  <si>
+    <t>IMT2</t>
+  </si>
+  <si>
+    <t>IMT3</t>
+  </si>
+  <si>
+    <t>IMU</t>
+  </si>
+  <si>
+    <t>IMU2</t>
+  </si>
+  <si>
+    <t>IMU3</t>
+  </si>
+  <si>
+    <t>IOMC</t>
+  </si>
+  <si>
+    <t>ISBD</t>
+  </si>
+  <si>
+    <t>ISBH</t>
+  </si>
+  <si>
+    <t>MAG</t>
+  </si>
+  <si>
+    <t>MAG2</t>
+  </si>
+  <si>
+    <t>MAG3</t>
+  </si>
+  <si>
+    <t>MAV</t>
+  </si>
+  <si>
+    <t>MAVC</t>
+  </si>
+  <si>
+    <t>MODE</t>
+  </si>
+  <si>
+    <t>MSG</t>
+  </si>
+  <si>
+    <t>MULT</t>
+  </si>
+  <si>
+    <t>NK11</t>
+  </si>
+  <si>
+    <t>NK12</t>
+  </si>
+  <si>
+    <t>NK13</t>
+  </si>
+  <si>
+    <t>NK14</t>
+  </si>
+  <si>
+    <t>NKF0</t>
+  </si>
+  <si>
+    <t>NKF1</t>
+  </si>
+  <si>
+    <t>NKF2</t>
+  </si>
+  <si>
+    <t>NKF3</t>
+  </si>
+  <si>
+    <t>NKF4</t>
+  </si>
+  <si>
+    <t>NKF5</t>
+  </si>
+  <si>
+    <t>NKF6</t>
+  </si>
+  <si>
+    <t>NKF7</t>
+  </si>
+  <si>
+    <t>NKF8</t>
+  </si>
+  <si>
+    <t>NKF9</t>
+  </si>
+  <si>
+    <t>NKQ1</t>
+  </si>
+  <si>
+    <t>NKQ2</t>
+  </si>
+  <si>
+    <t>NKQ3</t>
+  </si>
+  <si>
+    <t>NKT1</t>
+  </si>
+  <si>
+    <t>NKT2</t>
+  </si>
+  <si>
+    <t>NTUN</t>
+  </si>
+  <si>
+    <t>OABR</t>
+  </si>
+  <si>
+    <t>OADJ</t>
+  </si>
+  <si>
+    <t>OF</t>
+  </si>
+  <si>
+    <t>ORGN</t>
+  </si>
+  <si>
+    <t>PARM</t>
+  </si>
+  <si>
+    <t>PIDA</t>
+  </si>
+  <si>
+    <t>PIDP</t>
+  </si>
+  <si>
+    <t>PIDR</t>
+  </si>
+  <si>
+    <t>PIDS</t>
+  </si>
+  <si>
+    <t>PIDY</t>
+  </si>
+  <si>
+    <t>PIQA</t>
+  </si>
+  <si>
+    <t>PIQP</t>
+  </si>
+  <si>
+    <t>PIQR</t>
+  </si>
+  <si>
+    <t>PIQY</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>POWR</t>
+  </si>
+  <si>
+    <t>PRX</t>
+  </si>
+  <si>
+    <t>QTUN</t>
+  </si>
+  <si>
+    <t>RAD</t>
+  </si>
+  <si>
+    <t>RALY</t>
+  </si>
+  <si>
+    <t>RATE</t>
+  </si>
+  <si>
+    <t>RCIN</t>
+  </si>
+  <si>
+    <t>RCOU</t>
+  </si>
+  <si>
+    <t>RFND</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>RSSI</t>
+  </si>
+  <si>
+    <t>SBFE</t>
+  </si>
+  <si>
+    <t>SBPH</t>
+  </si>
+  <si>
+    <t>SBRE</t>
+  </si>
+  <si>
+    <t>SBRH</t>
+  </si>
+  <si>
+    <t>SBRM</t>
+  </si>
+  <si>
+    <t>SIM</t>
+  </si>
+  <si>
+    <t>SONR</t>
+  </si>
+  <si>
+    <t>SRTL</t>
+  </si>
+  <si>
+    <t>STAT</t>
+  </si>
+  <si>
+    <t>STRT</t>
+  </si>
+  <si>
+    <t>TEC2</t>
+  </si>
+  <si>
+    <t>TECS</t>
+  </si>
+  <si>
+    <t>TERR</t>
+  </si>
+  <si>
+    <t>TRIG</t>
+  </si>
+  <si>
+    <t>UBX1</t>
+  </si>
+  <si>
+    <t>UBX2</t>
+  </si>
+  <si>
+    <t>UBY1</t>
+  </si>
+  <si>
+    <t>UBY2</t>
+  </si>
+  <si>
+    <t>UNIT</t>
+  </si>
+  <si>
+    <t>VIBE</t>
+  </si>
+  <si>
+    <t>VISO</t>
+  </si>
+  <si>
+    <t>WENC</t>
+  </si>
+  <si>
+    <t>XK11</t>
+  </si>
+  <si>
+    <t>XK12</t>
+  </si>
+  <si>
+    <t>XK13</t>
+  </si>
+  <si>
+    <t>XK14</t>
+  </si>
+  <si>
+    <t>XKF0</t>
+  </si>
+  <si>
+    <t>XKF1</t>
+  </si>
+  <si>
+    <t>XKF2</t>
+  </si>
+  <si>
+    <t>XKF3</t>
+  </si>
+  <si>
+    <t>XKF4</t>
+  </si>
+  <si>
+    <t>XKF5</t>
+  </si>
+  <si>
+    <t>XKF6</t>
+  </si>
+  <si>
+    <t>XKF7</t>
+  </si>
+  <si>
+    <t>XKF8</t>
+  </si>
+  <si>
+    <t>XKF9</t>
+  </si>
+  <si>
+    <t>XKFD</t>
+  </si>
+  <si>
+    <t>XKQ1</t>
+  </si>
+  <si>
+    <t>XKQ2</t>
+  </si>
+  <si>
+    <t>XKQ3</t>
+  </si>
+  <si>
+    <t>XKV1</t>
+  </si>
+  <si>
+    <t>XKV2</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> µs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rad/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> m/s/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> degC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mGauss</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> m/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> m</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> V</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UNKNOWN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3600 W.s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ohm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> instance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> deg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> degheading</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> deg/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> deglatitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> deglongitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cm/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> us</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> satellites</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> d%</t>
+  </si>
+  <si>
+    <t>Messages</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>msg.fmt.units</t>
+  </si>
+  <si>
+    <t>"µs": 1.0,</t>
+  </si>
+  <si>
+    <t>"3600 W.s": 1.0,</t>
+  </si>
+  <si>
+    <t>"A": 1.0,</t>
+  </si>
+  <si>
+    <t>"B": 1.0,</t>
+  </si>
+  <si>
+    <t>"cm": 1.0,</t>
+  </si>
+  <si>
+    <t>"cm/s": 1.0,</t>
+  </si>
+  <si>
+    <t>"d%": 1.0,</t>
+  </si>
+  <si>
+    <t>"deg": 1.0,</t>
+  </si>
+  <si>
+    <t>"deg/s": 1.0,</t>
+  </si>
+  <si>
+    <t>"degC": 1.0,</t>
+  </si>
+  <si>
+    <t>"degheading": 1.0,</t>
+  </si>
+  <si>
+    <t>"deglatitude": 1.0,</t>
+  </si>
+  <si>
+    <t>"deglongitude": 1.0,</t>
+  </si>
+  <si>
+    <t>"Hz": 1.0,</t>
+  </si>
+  <si>
+    <t>"instance": 1.0,</t>
+  </si>
+  <si>
+    <t>"m": 1.0,</t>
+  </si>
+  <si>
+    <t>"m/s": 1.0,</t>
+  </si>
+  <si>
+    <t>"m/s/s": 1.0,</t>
+  </si>
+  <si>
+    <t>"mGauss": 1.0,</t>
+  </si>
+  <si>
+    <t>"ms": 1.0,</t>
+  </si>
+  <si>
+    <t>"Ohm": 1.0,</t>
+  </si>
+  <si>
+    <t>"Pa": 1.0,</t>
+  </si>
+  <si>
+    <t>"rad": 1.0,</t>
+  </si>
+  <si>
+    <t>"rad/s": 1.0,</t>
+  </si>
+  <si>
+    <t>"satellites": 1.0,</t>
+  </si>
+  <si>
+    <t>"UNKNOWN": 1.0,</t>
+  </si>
+  <si>
+    <t>"us": 1.0,</t>
+  </si>
+  <si>
+    <t>"V": 1.0,</t>
   </si>
 </sst>
 </file>
@@ -323,9 +1029,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7BC147E-106F-4A4B-91F1-8923A8931184}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G65"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1852,189 +2568,1748 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F68BF6-2F2F-41E5-B953-CF33EA178A7E}">
-  <dimension ref="A1:A34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE5B301-94F7-4E25-BCA8-093551E61F75}">
+  <dimension ref="A1:K177"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A34"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="4"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="E1" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="4">
+        <v>193</v>
+      </c>
+      <c r="E3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G3" t="str">
+        <f>_xlfn.CONCAT(CHAR(34),$E3,CHAR(34),": 1.0",",")</f>
+        <v>" µs": 1.0,</v>
+      </c>
+      <c r="K3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="4">
+        <v>194</v>
+      </c>
+      <c r="E4" t="s">
+        <v>271</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" ref="G4:G30" si="0">_xlfn.CONCAT(CHAR(34),$E4,CHAR(34),": 1.0",",")</f>
+        <v>" 3600 W.s": 1.0,</v>
+      </c>
+      <c r="K4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="4">
+        <v>195</v>
+      </c>
+      <c r="E5" t="s">
+        <v>269</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>" A": 1.0,</v>
+      </c>
+      <c r="K5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="4">
+        <v>250</v>
+      </c>
+      <c r="E6" t="s">
+        <v>257</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>" B": 1.0,</v>
+      </c>
+      <c r="K6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="4">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>280</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>" cm": 1.0,</v>
+      </c>
+      <c r="K7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="4">
+        <v>141</v>
+      </c>
+      <c r="E8" t="s">
+        <v>281</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>" cm/s": 1.0,</v>
+      </c>
+      <c r="K8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="4">
+        <v>236</v>
+      </c>
+      <c r="E9" t="s">
+        <v>284</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>" d%": 1.0,</v>
+      </c>
+      <c r="K9" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="4">
+        <v>251</v>
+      </c>
+      <c r="E10" t="s">
+        <v>274</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>" deg": 1.0,</v>
+      </c>
+      <c r="K10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="4">
+        <v>165</v>
+      </c>
+      <c r="E11" t="s">
+        <v>276</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>" deg/s": 1.0,</v>
+      </c>
+      <c r="K11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="4">
+        <v>243</v>
+      </c>
+      <c r="E12" t="s">
+        <v>261</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>" degC": 1.0,</v>
+      </c>
+      <c r="K12" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="4">
+        <v>146</v>
+      </c>
+      <c r="E13" t="s">
+        <v>275</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>" degheading": 1.0,</v>
+      </c>
+      <c r="K13" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="4">
+        <v>166</v>
+      </c>
+      <c r="E14" t="s">
+        <v>278</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>" deglatitude": 1.0,</v>
+      </c>
+      <c r="K14" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="4">
+        <v>164</v>
+      </c>
+      <c r="E15" t="s">
+        <v>279</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>" deglongitude": 1.0,</v>
+      </c>
+      <c r="K15" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="4">
+        <v>216</v>
+      </c>
+      <c r="E16" t="s">
+        <v>262</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>" Hz": 1.0,</v>
+      </c>
+      <c r="K16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="4">
+        <v>139</v>
+      </c>
+      <c r="E17" t="s">
+        <v>273</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>" instance": 1.0,</v>
+      </c>
+      <c r="K17" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="4">
+        <v>167</v>
+      </c>
+      <c r="E18" t="s">
+        <v>266</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>" m": 1.0,</v>
+      </c>
+      <c r="K18" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="4">
+        <v>168</v>
+      </c>
+      <c r="E19" t="s">
+        <v>264</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>" m/s": 1.0,</v>
+      </c>
+      <c r="K19" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="4">
+        <v>169</v>
+      </c>
+      <c r="E20" t="s">
+        <v>260</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>" m/s/s": 1.0,</v>
+      </c>
+      <c r="K20" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="4">
+        <v>170</v>
+      </c>
+      <c r="E21" t="s">
+        <v>263</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>" mGauss": 1.0,</v>
+      </c>
+      <c r="K21" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="4">
+        <v>171</v>
+      </c>
+      <c r="E22" t="s">
+        <v>267</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>" ms": 1.0,</v>
+      </c>
+      <c r="K22" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="4">
+        <v>172</v>
+      </c>
+      <c r="E23" t="s">
+        <v>272</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>" Ohm": 1.0,</v>
+      </c>
+      <c r="K23" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="4">
+        <v>173</v>
+      </c>
+      <c r="E24" t="s">
+        <v>265</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>" Pa": 1.0,</v>
+      </c>
+      <c r="K24" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="4">
+        <v>174</v>
+      </c>
+      <c r="E25" t="s">
+        <v>277</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>" rad": 1.0,</v>
+      </c>
+      <c r="K25" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="4">
+        <v>175</v>
+      </c>
+      <c r="E26" t="s">
+        <v>259</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>" rad/s": 1.0,</v>
+      </c>
+      <c r="K26" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="4">
+        <v>176</v>
+      </c>
+      <c r="E27" t="s">
+        <v>283</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>" satellites": 1.0,</v>
+      </c>
+      <c r="K27" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="4">
+        <v>177</v>
+      </c>
+      <c r="E28" t="s">
+        <v>270</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>" UNKNOWN": 1.0,</v>
+      </c>
+      <c r="K28" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="4">
+        <v>178</v>
+      </c>
+      <c r="E29" t="s">
+        <v>282</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>" us": 1.0,</v>
+      </c>
+      <c r="K29" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="4">
+        <v>179</v>
+      </c>
+      <c r="E30" t="s">
+        <v>268</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>" V": 1.0,</v>
+      </c>
+      <c r="K30" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="4">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" s="4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="4">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="4">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" s="4">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="4">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="4">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" s="4">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="4">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="4">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="4">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="4">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B45" s="4">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" s="4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B47" s="4">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B48" s="4">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="4">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="4">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="4">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B52" s="4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B53" s="4">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B54" s="4">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B55" s="4">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B56" s="4">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B57" s="4">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B58" s="4">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B59" s="4">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B60" s="4">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B61" s="4">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62" s="4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B63" s="4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B64" s="4">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B65" s="4">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B66" s="4">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B67" s="4">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B68" s="4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B69" s="4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B70" s="4">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B71" s="4">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="4">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B73" s="4">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B74" s="4">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B75" s="4">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B76" s="4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" s="4">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B78" s="4">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" s="4">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B80" s="4">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B81" s="4">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B82" s="4">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B83" s="4">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B84" s="4">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B85" s="4">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B86" s="4">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B87" s="4">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B88" s="4">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B89" s="4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B90" s="4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B91" s="4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B92" s="4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B93" s="4">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B94" s="4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B95" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B96" s="4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B97" s="4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B98" s="4">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B99" s="4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B100" s="4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B101" s="4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B102" s="4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B103" s="4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B104" s="4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B105" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B106" s="4">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B107" s="4">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B108" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B109" s="4">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B110" s="4">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B111" s="4">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B112" s="4">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B113" s="4">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B114" s="4">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B115" s="4">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B116" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B117" s="4">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B118" s="4">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B119" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B120" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B121" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B122" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B123" s="4">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B124" s="4">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B125" s="4">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B126" s="4">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B127" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B128" s="4">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B129" s="4">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B130" s="4">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B131" s="4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B132" s="4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B133" s="4">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B134" s="4">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B135" s="4">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B136" s="4">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B137" s="4">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B138" s="4">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B139" s="4">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B140" s="4">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B141" s="4">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B142" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B143" s="4">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B144" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B145" s="4">
         <v>2</v>
       </c>
     </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B146" s="4">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B147" s="4">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B148" s="4">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B149" s="4">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B150" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B151" s="4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B152" s="4">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B153" s="4">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B154" s="4">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B155" s="4">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B156" s="4">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B157" s="4">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B158" s="4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B159" s="4">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B160" s="4">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B161" s="4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B162" s="4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B163" s="4">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B164" s="4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B165" s="4">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B166" s="4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B167" s="4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B168" s="4">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B169" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B170" s="4">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B171" s="4">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B172" s="4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B173" s="4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B174" s="4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B175" s="4">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B176" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B177" s="4">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B355">
+    <sortCondition ref="A3:A355"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B54E11F8-2B15-4BD1-9DDA-003D0E7E0B14}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A31">
+    <sortCondition ref="A2:A31"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>